<commit_message>
static GRADE is string now, added functions for grade`s processing
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init_new.xlsx
+++ b/src/main/resources/xlsx/init_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Russian1</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Class</t>
+  </si>
+  <si>
+    <t>1а</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,8 +523,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,8 +537,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <v>2</v>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,8 +551,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,8 +565,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,8 +579,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>2</v>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,8 +593,8 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,8 +607,8 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,8 +621,8 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,8 +635,8 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,8 +649,8 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,8 +663,8 @@
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,8 +677,8 @@
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,8 +691,8 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,8 +705,8 @@
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,8 +719,8 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="2">
-        <v>1</v>
+      <c r="D18" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,8 +733,8 @@
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="2">
-        <v>1</v>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,8 +747,8 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21" s="2">
-        <v>1</v>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,8 +761,8 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22" s="2">
-        <v>1</v>
+      <c r="D22" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -772,8 +775,8 @@
       <c r="C23">
         <v>4</v>
       </c>
-      <c r="D23" s="2">
-        <v>1</v>
+      <c r="D23" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,8 +789,8 @@
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="D25" s="2">
-        <v>1</v>
+      <c r="D25" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,8 +803,8 @@
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" s="2">
-        <v>1</v>
+      <c r="D26" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,8 +817,8 @@
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27" s="2">
-        <v>1</v>
+      <c r="D27" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,8 +831,8 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28" s="2">
-        <v>1</v>
+      <c r="D28" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create timetable from new excel
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init_new.xlsx
+++ b/src/main/resources/xlsx/init_new.xlsx
@@ -24,114 +24,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
-  <si>
-    <t>Russian1</t>
-  </si>
-  <si>
-    <t>Russian3</t>
-  </si>
-  <si>
-    <t>Russian5</t>
-  </si>
-  <si>
-    <t>Math1</t>
-  </si>
-  <si>
-    <t>Phys1</t>
-  </si>
-  <si>
-    <t>Litr1</t>
-  </si>
-  <si>
-    <t>English1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>№ lesson</t>
+  </si>
+  <si>
+    <t>Day of the week</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
   <si>
     <t>placeholder</t>
   </si>
   <si>
-    <t>Math2</t>
-  </si>
-  <si>
-    <t>English2</t>
-  </si>
-  <si>
-    <t>Phys2</t>
-  </si>
-  <si>
-    <t>Phys3</t>
-  </si>
-  <si>
-    <t>Phys4</t>
-  </si>
-  <si>
-    <t>Phys5</t>
-  </si>
-  <si>
-    <t>English3</t>
-  </si>
-  <si>
-    <t>Litra3</t>
-  </si>
-  <si>
-    <t>Math4</t>
-  </si>
-  <si>
-    <t>English4</t>
-  </si>
-  <si>
-    <t>Math5</t>
-  </si>
-  <si>
-    <t>1,2,5</t>
-  </si>
-  <si>
-    <t>1-2,5</t>
-  </si>
-  <si>
-    <t>1-2,4-5</t>
-  </si>
-  <si>
-    <t>2-5</t>
-  </si>
-  <si>
-    <t>3,4</t>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Михайлова</t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>5а-9а,5б-9б</t>
+  </si>
+  <si>
+    <t>Платунова</t>
   </si>
   <si>
     <t>1-5</t>
   </si>
   <si>
-    <t>1-2,4</t>
+    <t>10а-11а,10б-11б,8в</t>
+  </si>
+  <si>
+    <t>Кузнецова</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>5а,5б,9а-10а,9б,9в</t>
+  </si>
+  <si>
+    <t>Автономова</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>7а,7б,7в</t>
+  </si>
+  <si>
+    <t>Калинина</t>
+  </si>
+  <si>
+    <t>5в-6в,6а</t>
+  </si>
+  <si>
+    <t>Реппо</t>
+  </si>
+  <si>
+    <t>5а-6а,5в-6в,6б,8в</t>
+  </si>
+  <si>
+    <t>Кузьмина</t>
+  </si>
+  <si>
+    <t>10а-11а,10б-11б,7в</t>
+  </si>
+  <si>
+    <t>Степанян</t>
+  </si>
+  <si>
+    <t>11а,11б,10б,9а,9б,9в</t>
+  </si>
+  <si>
+    <t>Григорьева</t>
+  </si>
+  <si>
+    <t>7а,8б,7б,6в,,8а</t>
+  </si>
+  <si>
+    <t>Кузикова</t>
   </si>
   <si>
     <t>1-3</t>
   </si>
   <si>
-    <t>1,3,5</t>
-  </si>
-  <si>
-    <t>4-5</t>
-  </si>
-  <si>
-    <t>2-4</t>
-  </si>
-  <si>
-    <t>1,3</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>№ lesson</t>
-  </si>
-  <si>
-    <t>Day of the week</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>1а</t>
+    <t>5б</t>
+  </si>
+  <si>
+    <t>Селькин</t>
+  </si>
+  <si>
+    <t>6а,6б,6в</t>
+  </si>
+  <si>
+    <t>Орлова</t>
+  </si>
+  <si>
+    <t>9б,6в,6б,7а,8б,8а,11б</t>
   </si>
 </sst>
 </file>
@@ -486,353 +486,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E1" sqref="E1:AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25">
         <v>5</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added field subjectName to Teacher objects
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init_new.xlsx
+++ b/src/main/resources/xlsx/init_new.xlsx
@@ -209,10 +209,10 @@
     <t>Английский</t>
   </si>
   <si>
-    <t>Изо</t>
-  </si>
-  <si>
     <t>География</t>
+  </si>
+  <si>
+    <t>ИЗО</t>
   </si>
 </sst>
 </file>
@@ -569,9 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150:XFD150"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1011,7 +1009,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>41</v>
@@ -1028,7 +1026,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>43</v>
@@ -1045,7 +1043,7 @@
         <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>10</v>
@@ -1062,7 +1060,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>38</v>
@@ -1490,7 +1488,7 @@
         <v>40</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>41</v>
@@ -1507,7 +1505,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>43</v>
@@ -1524,7 +1522,7 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>10</v>
@@ -1541,7 +1539,7 @@
         <v>37</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>38</v>
@@ -1969,7 +1967,7 @@
         <v>40</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>41</v>
@@ -1986,7 +1984,7 @@
         <v>42</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>43</v>
@@ -2003,7 +2001,7 @@
         <v>44</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>10</v>
@@ -2020,7 +2018,7 @@
         <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>38</v>
@@ -2448,7 +2446,7 @@
         <v>40</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>41</v>
@@ -2465,7 +2463,7 @@
         <v>42</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>43</v>
@@ -2482,7 +2480,7 @@
         <v>44</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>10</v>
@@ -2499,7 +2497,7 @@
         <v>37</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>38</v>
@@ -2927,7 +2925,7 @@
         <v>40</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>41</v>
@@ -2944,7 +2942,7 @@
         <v>42</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>43</v>
@@ -2961,7 +2959,7 @@
         <v>44</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>10</v>
@@ -2978,7 +2976,7 @@
         <v>37</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
seems like daily limits finally work
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init_new.xlsx
+++ b/src/main/resources/xlsx/init_new.xlsx
@@ -569,7 +569,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1063,7 +1065,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
now daily limits FINALLY work
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init_new.xlsx
+++ b/src/main/resources/xlsx/init_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="65">
   <si>
     <t>Subject</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>ИЗО</t>
+  </si>
+  <si>
+    <t>3-6</t>
+  </si>
+  <si>
+    <t>1,6</t>
   </si>
 </sst>
 </file>
@@ -229,12 +235,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -249,10 +261,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -569,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,20 +2529,20 @@
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="122" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="1" t="s">
+      <c r="C122" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E122" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2633,20 +2648,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="129" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D129" s="1" t="s">
+      <c r="C129" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E129" s="2" t="s">
+      <c r="E129" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2701,20 +2716,20 @@
         <v>46</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="133" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D133" s="1" t="s">
+      <c r="C133" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E133" s="2" t="s">
+      <c r="E133" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2735,71 +2750,71 @@
         <v>45</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="135" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D135" s="1" t="s">
+      <c r="C135" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E135" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="E135" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D136" s="1" t="s">
+      <c r="C136" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E136" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="E136" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D137" s="1" t="s">
+      <c r="C137" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="E137" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D138" s="1" t="s">
+      <c r="C138" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D138" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E138" s="2" t="s">
+      <c r="E138" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2820,71 +2835,71 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="140" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D140" s="1" t="s">
+      <c r="C140" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D140" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E140" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="E140" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D141" s="1" t="s">
+      <c r="C141" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D141" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E141" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="E141" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D142" s="1" t="s">
+      <c r="C142" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D142" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E142" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="E142" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D143" s="1" t="s">
+      <c r="C143" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D143" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E143" s="2" t="s">
+      <c r="E143" s="5" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit before adding new list to writer
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init_new.xlsx
+++ b/src/main/resources/xlsx/init_new.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The Diamond Doge\IdeaProjects\GA\src\main\resources\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiksanov\IdeaProjects\GA\src\main\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="112">
   <si>
     <t>Subject</t>
   </si>
@@ -357,12 +357,15 @@
   </si>
   <si>
     <t>5б-6б,7а,7б,8в</t>
+  </si>
+  <si>
+    <t>№ lesson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -720,16 +723,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" style="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>

</xml_diff>